<commit_message>
Complete "Take conditional formatting to the next level"
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/10 - 使用条件格式.xlsx
+++ b/Excel动手实验室 - 材料/10 - 使用条件格式.xlsx
@@ -263,7 +263,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -349,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1">
@@ -363,27 +363,7 @@
     <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -676,6 +656,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
+    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Fix the error of material in 10
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/10 - 使用条件格式.xlsx
+++ b/Excel动手实验室 - 材料/10 - 使用条件格式.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="347" windowWidth="18434" windowHeight="8097"/>
   </bookViews>
   <sheets>
     <sheet name="条件格式" sheetId="1" r:id="rId1"/>
@@ -263,13 +263,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -277,14 +277,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -293,7 +293,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -349,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1">
@@ -654,10 +654,10 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="1" max="1" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -810,12 +810,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="15.73046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -831,7 +833,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="4">
-        <v>41828</v>
+        <v>42193</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -839,7 +841,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="4">
-        <v>41863</v>
+        <v>42228</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -847,7 +849,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="4">
-        <v>41835</v>
+        <v>42200</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -855,7 +857,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="4">
-        <v>41847</v>
+        <v>42212</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -863,7 +865,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="4">
-        <v>41855</v>
+        <v>42220</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -871,7 +873,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="4">
-        <v>41843</v>
+        <v>42208</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -879,7 +881,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="4">
-        <v>41844</v>
+        <v>42209</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -887,7 +889,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="4">
-        <v>41855</v>
+        <v>42220</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -895,7 +897,7 @@
         <v>32</v>
       </c>
       <c r="B10" s="4">
-        <v>41865</v>
+        <v>42230</v>
       </c>
     </row>
   </sheetData>
@@ -908,12 +910,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -944,7 +948,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="4">
-        <v>41785</v>
+        <v>42150</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>39</v>
@@ -961,7 +965,7 @@
         <v>41</v>
       </c>
       <c r="D3" s="4">
-        <v>41792</v>
+        <v>42157</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>42</v>
@@ -978,7 +982,7 @@
         <v>41</v>
       </c>
       <c r="D4" s="4">
-        <v>41672</v>
+        <v>42037</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>44</v>
@@ -995,7 +999,7 @@
         <v>46</v>
       </c>
       <c r="D5" s="4">
-        <v>41832</v>
+        <v>42197</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>39</v>
@@ -1012,7 +1016,7 @@
         <v>48</v>
       </c>
       <c r="D6" s="4">
-        <v>41726</v>
+        <v>42091</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>49</v>
@@ -1029,7 +1033,7 @@
         <v>50</v>
       </c>
       <c r="D7" s="4">
-        <v>41757</v>
+        <v>42122</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>51</v>
@@ -1046,7 +1050,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="4">
-        <v>41792</v>
+        <v>42157</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>54</v>
@@ -1063,7 +1067,7 @@
         <v>38</v>
       </c>
       <c r="D9" s="4">
-        <v>41726</v>
+        <v>42091</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>54</v>
@@ -1080,7 +1084,7 @@
         <v>57</v>
       </c>
       <c r="D10" s="4">
-        <v>41798</v>
+        <v>42163</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>58</v>
@@ -1098,9 +1102,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>